<commit_message>
Agregar Percepcion y deduccion
Solo jala agregar por empleado, falta por departamento
</commit_message>
<xml_diff>
--- a/Excel/Deducciones.xlsx
+++ b/Excel/Deducciones.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25128"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Escuela documentos\semestre 6\MAD\proyecto\Proyecto MAD\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C9EA01B-EF31-43C9-BBDE-BED58E4AF086}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66BFEAB6-4DDA-46A7-BA40-5F6D1DE083F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7185" yWindow="2025" windowWidth="11520" windowHeight="7965" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -25,12 +25,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>Nombre</t>
-  </si>
-  <si>
-    <t>Fecha</t>
   </si>
   <si>
     <t>Porcentaje</t>
@@ -87,9 +84,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -370,10 +366,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -384,59 +380,47 @@
     <col min="4" max="4" width="10.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>3</v>
       </c>
-      <c r="D1" t="s">
-        <v>2</v>
+      <c r="B2">
+        <v>84.5</v>
+      </c>
+      <c r="C2">
+        <v>0.9</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="1">
-        <v>44679</v>
-      </c>
-      <c r="C2">
-        <v>84.5</v>
-      </c>
-      <c r="D2">
-        <v>0.9</v>
+      <c r="B3">
+        <v>95.62</v>
+      </c>
+      <c r="C3">
+        <v>0.5</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="1">
-        <v>44680</v>
-      </c>
-      <c r="C3">
-        <v>95.62</v>
-      </c>
-      <c r="D3">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="1">
-        <v>44681</v>
+      <c r="B4">
+        <v>50</v>
       </c>
       <c r="C4">
-        <v>50</v>
-      </c>
-      <c r="D4">
         <v>0.5</v>
       </c>
     </row>

</xml_diff>